<commit_message>
#update approval screen prod/15671-Settlement-Update-Beneficiary-And-Add-General-Preview
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
@@ -42,328 +42,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alex Phuong</author>
-  </authors>
-  <commentList>
-    <comment ref="H12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-số Settlement No</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Request Date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Requester Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Requester Department</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Description + Payee Name EN</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Bank Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Banks Account</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Beneficiary Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Description</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Settlement Total Amount</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G40" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Amount</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B42" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Amout số tiền bằng chứ</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
@@ -530,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0.00_);_([$VND]\ * \(#,##0.00\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -569,19 +247,6 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1314,7 +979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1706,6 +1371,5 @@
   <pageMargins left="0.5" right="0.4" top="0.28999999999999998" bottom="0.28999999999999998" header="0.3" footer="0.3"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug create invoice from Bravo
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynne.loc\Desktop\eFMSSource\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\SettlePayment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\SettlePayment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ĐƠN VỊ:…………………………………………………………………………………….</t>
   </si>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0.00_);_([$VND]\ * \(#,##0.00\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$USD]\ * #,##0.00_);_([$USD]\ * \(#,##0.00\);_([$USD]\ * &quot;-&quot;??_);_(@_)"/>
@@ -982,8 +982,8 @@
   </sheetPr>
   <dimension ref="A10:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1348,11 +1348,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="56" spans="1:1" s="3" customFormat="1">
       <c r="A56" s="35"/>
     </row>

</xml_diff>

<commit_message>
#update fix not view tick on preview
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>ĐƠN VỊ:…………………………………………………………………………………….</t>
   </si>
@@ -202,18 +202,6 @@
   </si>
   <si>
     <t>{Accountant}</t>
-  </si>
-  <si>
-    <t>{tick1}</t>
-  </si>
-  <si>
-    <t>{tick2}</t>
-  </si>
-  <si>
-    <t>{tick3}</t>
-  </si>
-  <si>
-    <t>{tick4}</t>
   </si>
   <si>
     <t>{SettlementNote}</t>
@@ -648,36 +636,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,10 +1081,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="42"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1157,18 +1145,18 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.75" customHeight="1">
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" ht="24.75" customHeight="1">
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="24.75" customHeight="1">
       <c r="E24" s="14" t="s">
@@ -1192,11 +1180,11 @@
       <c r="E26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46" t="s">
+      <c r="G26" s="50"/>
+      <c r="H26" s="51" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1212,7 +1200,7 @@
       <c r="G27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="47"/>
+      <c r="H27" s="52"/>
     </row>
     <row r="28" spans="1:8" ht="21" customHeight="1">
       <c r="A28" s="21"/>
@@ -1229,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
@@ -1374,8 +1362,8 @@
       <c r="B42" s="3"/>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="13">
-      <c r="A44" s="51"/>
-      <c r="B44" s="51" t="s">
+      <c r="A44" s="42"/>
+      <c r="B44" s="42" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1407,33 +1395,25 @@
     </row>
     <row r="46" spans="1:9" ht="51.5" customHeight="1">
       <c r="A46" s="40"/>
-      <c r="B46" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G46" s="48"/>
-      <c r="H46" s="41" t="s">
-        <v>53</v>
-      </c>
+      <c r="B46" s="40"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="41"/>
       <c r="I46" s="40"/>
     </row>
     <row r="47" spans="1:9" ht="12.5" customHeight="1">
-      <c r="A47" s="52"/>
-      <c r="B47" s="52" t="s">
+      <c r="A47" s="43"/>
+      <c r="B47" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="49" t="s">
+      <c r="D47" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="49"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
       <c r="H47" s="39" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
#update office info with current office in templates adv/settle
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-General-Preview.xlsx
@@ -662,6 +662,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -694,9 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,40 +983,38 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="23.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1">
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
     </row>
     <row r="2" spans="1:10" ht="60" customHeight="1">
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="56"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
@@ -1025,7 +1023,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19.5" customHeight="1" thickBot="1"/>
-    <row r="12" spans="1:10" s="9" customFormat="1" ht="21.75" thickTop="1" thickBot="1">
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1058,10 +1056,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="50"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -1122,25 +1120,25 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.75" customHeight="1">
-      <c r="E22" s="51" t="s">
+      <c r="E22" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
     </row>
     <row r="23" spans="1:8" ht="24.75" customHeight="1">
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="24.75" customHeight="1">
       <c r="E24" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="25" spans="1:8" ht="13" thickBot="1"/>
     <row r="26" spans="1:8" s="17" customFormat="1" ht="40.5" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>11</v>
@@ -1157,11 +1155,11 @@
       <c r="E26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="54" t="s">
+      <c r="G26" s="54"/>
+      <c r="H26" s="55" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1177,7 +1175,7 @@
       <c r="G27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="55"/>
+      <c r="H27" s="56"/>
     </row>
     <row r="28" spans="1:8" ht="21" customHeight="1">
       <c r="A28" s="21"/>
@@ -1338,7 +1336,7 @@
       </c>
       <c r="B42" s="3"/>
     </row>
-    <row r="44" spans="1:9" s="1" customFormat="1">
+    <row r="44" spans="1:9" s="1" customFormat="1" ht="13">
       <c r="A44" s="42"/>
       <c r="B44" s="42" t="s">
         <v>21</v>
@@ -1354,7 +1352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="37" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:9" s="37" customFormat="1" ht="17.149999999999999" customHeight="1">
       <c r="B45" s="37" t="s">
         <v>25</v>
       </c>
@@ -1370,32 +1368,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="51.6" customHeight="1">
+    <row r="46" spans="1:9" ht="51.65" customHeight="1">
       <c r="A46" s="40"/>
       <c r="B46" s="40"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="41"/>
       <c r="I46" s="40"/>
     </row>
-    <row r="47" spans="1:9" ht="12.6" customHeight="1">
+    <row r="47" spans="1:9" ht="12.65" customHeight="1">
       <c r="A47" s="43"/>
       <c r="B47" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D47" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="48"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
       <c r="H47" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:1" s="3" customFormat="1">
+    <row r="56" spans="1:1" s="3" customFormat="1" ht="13">
       <c r="A56" s="34"/>
     </row>
   </sheetData>

</xml_diff>